<commit_message>
Added 8 new questions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HtmlAcademy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HtmlAcademy\FamilyFeud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494C3589-53A4-4C09-A13F-D20A0B699CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B267832-EA4C-4C7A-9D4E-4CD8CAB64C94}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="32914" windowHeight="17914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="32916" windowHeight="17916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformed by JSON-CSV.CO" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="305">
   <si>
     <t>Question</t>
   </si>
@@ -773,6 +773,168 @@
   </si>
   <si>
     <t>Носит чёрное</t>
+  </si>
+  <si>
+    <t>Туристы\экскурсия</t>
+  </si>
+  <si>
+    <t>Приёмная комиссия</t>
+  </si>
+  <si>
+    <t>Покупатели</t>
+  </si>
+  <si>
+    <t>Грабители</t>
+  </si>
+  <si>
+    <t>Жильцы</t>
+  </si>
+  <si>
+    <t>Повар</t>
+  </si>
+  <si>
+    <t>Врач</t>
+  </si>
+  <si>
+    <t>Банщик</t>
+  </si>
+  <si>
+    <t>Сардина</t>
+  </si>
+  <si>
+    <t>Сельдь</t>
+  </si>
+  <si>
+    <t>Горбуша</t>
+  </si>
+  <si>
+    <t>Скумбрия</t>
+  </si>
+  <si>
+    <t>Сайра</t>
+  </si>
+  <si>
+    <t>Килька</t>
+  </si>
+  <si>
+    <t>Метель</t>
+  </si>
+  <si>
+    <t>Мель</t>
+  </si>
+  <si>
+    <t>Ельник</t>
+  </si>
+  <si>
+    <t>Капель</t>
+  </si>
+  <si>
+    <t>Карусель</t>
+  </si>
+  <si>
+    <t>Мебель</t>
+  </si>
+  <si>
+    <t>Муку</t>
+  </si>
+  <si>
+    <t>Консервы</t>
+  </si>
+  <si>
+    <t>Крупу</t>
+  </si>
+  <si>
+    <t>Спички</t>
+  </si>
+  <si>
+    <t>Сахар</t>
+  </si>
+  <si>
+    <t>Соль</t>
+  </si>
+  <si>
+    <t>Детям</t>
+  </si>
+  <si>
+    <t>Пенсионерам</t>
+  </si>
+  <si>
+    <t>Безработным</t>
+  </si>
+  <si>
+    <t>Олигархам\богатым</t>
+  </si>
+  <si>
+    <t>Инвалидам</t>
+  </si>
+  <si>
+    <t>Домохозяйкам</t>
+  </si>
+  <si>
+    <t>Дом</t>
+  </si>
+  <si>
+    <t>Человек</t>
+  </si>
+  <si>
+    <t>Город</t>
+  </si>
+  <si>
+    <t>Язык</t>
+  </si>
+  <si>
+    <t>Родители</t>
+  </si>
+  <si>
+    <t>Ребёнок</t>
+  </si>
+  <si>
+    <t>Лошадь</t>
+  </si>
+  <si>
+    <t>Солдат</t>
+  </si>
+  <si>
+    <t>Слон</t>
+  </si>
+  <si>
+    <t>Цапля</t>
+  </si>
+  <si>
+    <t>Охранник</t>
+  </si>
+  <si>
+    <t>Корова</t>
+  </si>
+  <si>
+    <t>033. Пять человек осматривают здание. Кто они?</t>
+  </si>
+  <si>
+    <t>034. Кто на работе использует полотенце?</t>
+  </si>
+  <si>
+    <t>035. Из какой рыбы делают консервы?</t>
+  </si>
+  <si>
+    <t>036. В каких словах есть слово "ель"?</t>
+  </si>
+  <si>
+    <t>037. Какие продукты или товары покупают "про запас"?</t>
+  </si>
+  <si>
+    <t>038. Кому можно не работать?</t>
+  </si>
+  <si>
+    <t>039. Что может быть родным?</t>
+  </si>
+  <si>
+    <t>040. Кто спит стоя?</t>
+  </si>
+  <si>
+    <t>Строители\архитектор</t>
+  </si>
+  <si>
+    <t>Мопед</t>
   </si>
 </sst>
 </file>
@@ -1111,19 +1273,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C243"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="B243" sqref="B243"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="74.3046875" customWidth="1"/>
-    <col min="2" max="2" width="29.23046875" customWidth="1"/>
+    <col min="1" max="1" width="74.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1145,7 +1307,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -1153,7 +1315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -1161,7 +1323,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -1169,7 +1331,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1177,7 +1339,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -1185,7 +1347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -1204,7 +1366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>19</v>
       </c>
@@ -1212,7 +1374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>21</v>
       </c>
@@ -1220,7 +1382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -1228,7 +1390,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>25</v>
       </c>
@@ -1236,7 +1398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1247,7 +1409,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>29</v>
       </c>
@@ -1255,7 +1417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>31</v>
       </c>
@@ -1263,7 +1425,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -1271,7 +1433,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -1279,7 +1441,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -1287,7 +1449,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1298,7 +1460,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>39</v>
       </c>
@@ -1306,7 +1468,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>41</v>
       </c>
@@ -1314,7 +1476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>42</v>
       </c>
@@ -1322,7 +1484,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>44</v>
       </c>
@@ -1330,7 +1492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>45</v>
       </c>
@@ -1338,7 +1500,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1349,7 +1511,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>49</v>
       </c>
@@ -1357,7 +1519,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>51</v>
       </c>
@@ -1365,7 +1527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>52</v>
       </c>
@@ -1373,7 +1535,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>53</v>
       </c>
@@ -1381,7 +1543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>54</v>
       </c>
@@ -1389,7 +1551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1400,7 +1562,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>57</v>
       </c>
@@ -1408,7 +1570,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>59</v>
       </c>
@@ -1416,7 +1578,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>61</v>
       </c>
@@ -1424,7 +1586,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>62</v>
       </c>
@@ -1432,7 +1594,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>63</v>
       </c>
@@ -1440,7 +1602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -1451,7 +1613,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>67</v>
       </c>
@@ -1459,7 +1621,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>69</v>
       </c>
@@ -1467,7 +1629,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>70</v>
       </c>
@@ -1475,7 +1637,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>72</v>
       </c>
@@ -1483,7 +1645,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>74</v>
       </c>
@@ -1491,7 +1653,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>75</v>
       </c>
@@ -1502,7 +1664,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>78</v>
       </c>
@@ -1510,7 +1672,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>80</v>
       </c>
@@ -1518,7 +1680,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>81</v>
       </c>
@@ -1526,7 +1688,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>82</v>
       </c>
@@ -1534,7 +1696,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>83</v>
       </c>
@@ -1542,7 +1704,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>84</v>
       </c>
@@ -1553,7 +1715,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>87</v>
       </c>
@@ -1561,7 +1723,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>88</v>
       </c>
@@ -1569,7 +1731,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>90</v>
       </c>
@@ -1577,7 +1739,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>91</v>
       </c>
@@ -1585,7 +1747,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>92</v>
       </c>
@@ -1593,7 +1755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>93</v>
       </c>
@@ -1604,7 +1766,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>95</v>
       </c>
@@ -1612,7 +1774,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>97</v>
       </c>
@@ -1620,7 +1782,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>98</v>
       </c>
@@ -1628,7 +1790,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>99</v>
       </c>
@@ -1636,7 +1798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>100</v>
       </c>
@@ -1644,7 +1806,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>101</v>
       </c>
@@ -1655,7 +1817,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>104</v>
       </c>
@@ -1663,7 +1825,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>106</v>
       </c>
@@ -1671,7 +1833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>107</v>
       </c>
@@ -1679,7 +1841,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>108</v>
       </c>
@@ -1687,7 +1849,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>109</v>
       </c>
@@ -1695,7 +1857,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -1706,7 +1868,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>112</v>
       </c>
@@ -1714,7 +1876,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>113</v>
       </c>
@@ -1722,7 +1884,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>114</v>
       </c>
@@ -1730,7 +1892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>115</v>
       </c>
@@ -1738,7 +1900,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>116</v>
       </c>
@@ -1746,7 +1908,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>117</v>
       </c>
@@ -1757,7 +1919,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>120</v>
       </c>
@@ -1765,7 +1927,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>121</v>
       </c>
@@ -1773,7 +1935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>122</v>
       </c>
@@ -1781,7 +1943,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>123</v>
       </c>
@@ -1789,7 +1951,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>124</v>
       </c>
@@ -1797,7 +1959,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>125</v>
       </c>
@@ -1808,7 +1970,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>127</v>
       </c>
@@ -1816,7 +1978,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>128</v>
       </c>
@@ -1824,7 +1986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>129</v>
       </c>
@@ -1832,7 +1994,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>130</v>
       </c>
@@ -1840,7 +2002,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>131</v>
       </c>
@@ -1848,7 +2010,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>132</v>
       </c>
@@ -1859,7 +2021,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>134</v>
       </c>
@@ -1867,7 +2029,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>45</v>
       </c>
@@ -1875,7 +2037,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>137</v>
       </c>
@@ -1883,7 +2045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>138</v>
       </c>
@@ -1891,7 +2053,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>139</v>
       </c>
@@ -1899,7 +2061,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>140</v>
       </c>
@@ -1910,7 +2072,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>142</v>
       </c>
@@ -1918,7 +2080,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>144</v>
       </c>
@@ -1926,7 +2088,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>146</v>
       </c>
@@ -1934,7 +2096,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>147</v>
       </c>
@@ -1942,7 +2104,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>148</v>
       </c>
@@ -1950,7 +2112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>149</v>
       </c>
@@ -1961,7 +2123,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>151</v>
       </c>
@@ -1969,7 +2131,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>153</v>
       </c>
@@ -1977,7 +2139,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>154</v>
       </c>
@@ -1985,7 +2147,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>155</v>
       </c>
@@ -1993,7 +2155,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>156</v>
       </c>
@@ -2001,7 +2163,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>157</v>
       </c>
@@ -2012,7 +2174,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>159</v>
       </c>
@@ -2020,7 +2182,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>160</v>
       </c>
@@ -2028,7 +2190,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>161</v>
       </c>
@@ -2036,7 +2198,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>162</v>
       </c>
@@ -2044,7 +2206,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>163</v>
       </c>
@@ -2052,7 +2214,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>164</v>
       </c>
@@ -2060,7 +2222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>165</v>
       </c>
@@ -2071,7 +2233,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>167</v>
       </c>
@@ -2079,7 +2241,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>168</v>
       </c>
@@ -2087,7 +2249,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>169</v>
       </c>
@@ -2095,7 +2257,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>170</v>
       </c>
@@ -2103,7 +2265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>171</v>
       </c>
@@ -2111,7 +2273,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>172</v>
       </c>
@@ -2122,7 +2284,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>174</v>
       </c>
@@ -2130,7 +2292,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>175</v>
       </c>
@@ -2138,7 +2300,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>176</v>
       </c>
@@ -2146,7 +2308,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>177</v>
       </c>
@@ -2154,7 +2316,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>178</v>
       </c>
@@ -2162,7 +2324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>179</v>
       </c>
@@ -2173,7 +2335,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>181</v>
       </c>
@@ -2181,7 +2343,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>182</v>
       </c>
@@ -2189,7 +2351,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>183</v>
       </c>
@@ -2197,7 +2359,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
         <v>184</v>
       </c>
@@ -2205,7 +2367,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
         <v>185</v>
       </c>
@@ -2213,7 +2375,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>186</v>
       </c>
@@ -2224,7 +2386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>188</v>
       </c>
@@ -2232,7 +2394,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>189</v>
       </c>
@@ -2240,7 +2402,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>190</v>
       </c>
@@ -2248,7 +2410,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>191</v>
       </c>
@@ -2256,7 +2418,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>192</v>
       </c>
@@ -2264,7 +2426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>193</v>
       </c>
@@ -2275,7 +2437,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>195</v>
       </c>
@@ -2283,7 +2445,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>197</v>
       </c>
@@ -2291,7 +2453,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>198</v>
       </c>
@@ -2299,7 +2461,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>199</v>
       </c>
@@ -2307,7 +2469,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
         <v>200</v>
       </c>
@@ -2315,7 +2477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>201</v>
       </c>
@@ -2326,7 +2488,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
         <v>203</v>
       </c>
@@ -2334,7 +2496,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B143" t="s">
         <v>204</v>
       </c>
@@ -2342,7 +2504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B144" t="s">
         <v>205</v>
       </c>
@@ -2350,7 +2512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B145" t="s">
         <v>206</v>
       </c>
@@ -2358,7 +2520,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
         <v>207</v>
       </c>
@@ -2366,7 +2528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>208</v>
       </c>
@@ -2377,7 +2539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B148" t="s">
         <v>210</v>
       </c>
@@ -2385,7 +2547,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
         <v>211</v>
       </c>
@@ -2393,7 +2555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B150" t="s">
         <v>100</v>
       </c>
@@ -2401,7 +2563,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
         <v>212</v>
       </c>
@@ -2409,7 +2571,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>213</v>
       </c>
@@ -2420,7 +2582,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
         <v>216</v>
       </c>
@@ -2428,7 +2590,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B154" t="s">
         <v>218</v>
       </c>
@@ -2436,7 +2598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B155" t="s">
         <v>219</v>
       </c>
@@ -2444,7 +2606,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B156" t="s">
         <v>220</v>
       </c>
@@ -2452,7 +2614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B157" t="s">
         <v>221</v>
       </c>
@@ -2460,12 +2622,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B158" t="s">
+        <v>304</v>
+      </c>
       <c r="C158" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>222</v>
       </c>
@@ -2476,7 +2641,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B160" t="s">
         <v>216</v>
       </c>
@@ -2484,7 +2649,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
         <v>218</v>
       </c>
@@ -2492,7 +2657,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
         <v>219</v>
       </c>
@@ -2500,7 +2665,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B163" t="s">
         <v>220</v>
       </c>
@@ -2508,7 +2673,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
         <v>221</v>
       </c>
@@ -2516,7 +2681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>223</v>
       </c>
@@ -2527,7 +2692,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B166" t="s">
         <v>225</v>
       </c>
@@ -2535,7 +2700,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
         <v>226</v>
       </c>
@@ -2543,7 +2708,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B168" t="s">
         <v>228</v>
       </c>
@@ -2551,7 +2716,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B169" t="s">
         <v>59</v>
       </c>
@@ -2559,7 +2724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B170" t="s">
         <v>61</v>
       </c>
@@ -2567,7 +2732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B171" t="s">
         <v>229</v>
       </c>
@@ -2575,7 +2740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>230</v>
       </c>
@@ -2586,7 +2751,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B173" t="s">
         <v>232</v>
       </c>
@@ -2594,7 +2759,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B174" t="s">
         <v>233</v>
       </c>
@@ -2602,7 +2767,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B175" t="s">
         <v>234</v>
       </c>
@@ -2610,7 +2775,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B176" t="s">
         <v>194</v>
       </c>
@@ -2618,7 +2783,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B177" t="s">
         <v>235</v>
       </c>
@@ -2626,7 +2791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>236</v>
       </c>
@@ -2637,7 +2802,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B179" t="s">
         <v>232</v>
       </c>
@@ -2645,7 +2810,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B180" t="s">
         <v>233</v>
       </c>
@@ -2653,7 +2818,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B181" t="s">
         <v>234</v>
       </c>
@@ -2661,7 +2826,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B182" t="s">
         <v>194</v>
       </c>
@@ -2669,7 +2834,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B183" t="s">
         <v>235</v>
       </c>
@@ -2677,7 +2842,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>237</v>
       </c>
@@ -2688,7 +2853,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B185" t="s">
         <v>239</v>
       </c>
@@ -2696,7 +2861,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B186" t="s">
         <v>240</v>
       </c>
@@ -2704,7 +2869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B187" t="s">
         <v>241</v>
       </c>
@@ -2712,7 +2877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B188" t="s">
         <v>242</v>
       </c>
@@ -2720,7 +2885,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
         <v>243</v>
       </c>
@@ -2728,7 +2893,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>244</v>
       </c>
@@ -2739,7 +2904,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
         <v>246</v>
       </c>
@@ -2747,7 +2912,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B192" t="s">
         <v>247</v>
       </c>
@@ -2755,7 +2920,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
         <v>248</v>
       </c>
@@ -2763,7 +2928,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
         <v>249</v>
       </c>
@@ -2771,7 +2936,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B195" t="s">
         <v>250</v>
       </c>
@@ -2779,7 +2944,416 @@
         <v>46</v>
       </c>
     </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>295</v>
+      </c>
+      <c r="B196" t="s">
+        <v>251</v>
+      </c>
+      <c r="C196">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B197" t="s">
+        <v>252</v>
+      </c>
+      <c r="C197">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B198" t="s">
+        <v>253</v>
+      </c>
+      <c r="C198">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B199" t="s">
+        <v>303</v>
+      </c>
+      <c r="C199">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B200" t="s">
+        <v>254</v>
+      </c>
+      <c r="C200">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B201" t="s">
+        <v>255</v>
+      </c>
+      <c r="C201">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>296</v>
+      </c>
+      <c r="B202" t="s">
+        <v>256</v>
+      </c>
+      <c r="C202">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B203" t="s">
+        <v>118</v>
+      </c>
+      <c r="C203">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B204" t="s">
+        <v>257</v>
+      </c>
+      <c r="C204">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B205" t="s">
+        <v>133</v>
+      </c>
+      <c r="C205">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B206" t="s">
+        <v>57</v>
+      </c>
+      <c r="C206">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B207" t="s">
+        <v>258</v>
+      </c>
+      <c r="C207">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>297</v>
+      </c>
+      <c r="B208" t="s">
+        <v>259</v>
+      </c>
+      <c r="C208">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B209" t="s">
+        <v>260</v>
+      </c>
+      <c r="C209">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B210" t="s">
+        <v>261</v>
+      </c>
+      <c r="C210">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B211" t="s">
+        <v>262</v>
+      </c>
+      <c r="C211">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B212" t="s">
+        <v>263</v>
+      </c>
+      <c r="C212">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B213" t="s">
+        <v>264</v>
+      </c>
+      <c r="C213">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>298</v>
+      </c>
+      <c r="B214" t="s">
+        <v>265</v>
+      </c>
+      <c r="C214">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B215" t="s">
+        <v>266</v>
+      </c>
+      <c r="C215">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B216" t="s">
+        <v>267</v>
+      </c>
+      <c r="C216">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B217" t="s">
+        <v>268</v>
+      </c>
+      <c r="C217">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B218" t="s">
+        <v>269</v>
+      </c>
+      <c r="C218">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B219" t="s">
+        <v>270</v>
+      </c>
+      <c r="C219">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>299</v>
+      </c>
+      <c r="B220" t="s">
+        <v>271</v>
+      </c>
+      <c r="C220">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B221" t="s">
+        <v>272</v>
+      </c>
+      <c r="C221">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B222" t="s">
+        <v>273</v>
+      </c>
+      <c r="C222">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B223" t="s">
+        <v>274</v>
+      </c>
+      <c r="C223">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B224" t="s">
+        <v>275</v>
+      </c>
+      <c r="C224">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B225" t="s">
+        <v>276</v>
+      </c>
+      <c r="C225">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>300</v>
+      </c>
+      <c r="B226" t="s">
+        <v>277</v>
+      </c>
+      <c r="C226">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B227" t="s">
+        <v>278</v>
+      </c>
+      <c r="C227">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B228" t="s">
+        <v>279</v>
+      </c>
+      <c r="C228">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B229" t="s">
+        <v>280</v>
+      </c>
+      <c r="C229">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B230" t="s">
+        <v>281</v>
+      </c>
+      <c r="C230">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B231" t="s">
+        <v>282</v>
+      </c>
+      <c r="C231">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>301</v>
+      </c>
+      <c r="B232" t="s">
+        <v>283</v>
+      </c>
+      <c r="C232">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B233" t="s">
+        <v>284</v>
+      </c>
+      <c r="C233">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B234" t="s">
+        <v>285</v>
+      </c>
+      <c r="C234">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B235" t="s">
+        <v>286</v>
+      </c>
+      <c r="C235">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B236" t="s">
+        <v>287</v>
+      </c>
+      <c r="C236">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B237" t="s">
+        <v>288</v>
+      </c>
+      <c r="C237">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>302</v>
+      </c>
+      <c r="B238" t="s">
+        <v>289</v>
+      </c>
+      <c r="C238">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B239" t="s">
+        <v>290</v>
+      </c>
+      <c r="C239">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B240" t="s">
+        <v>291</v>
+      </c>
+      <c r="C240">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="241" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B241" t="s">
+        <v>292</v>
+      </c>
+      <c r="C241">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="242" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B242" t="s">
+        <v>293</v>
+      </c>
+      <c r="C242">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="243" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B243" t="s">
+        <v>294</v>
+      </c>
+      <c r="C243">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>